<commit_message>
Add fresh templates ahead of stats exam 3
</commit_message>
<xml_diff>
--- a/Stats/Excel/Templates/Confidence Interval for One Proportion.xlsx
+++ b/Stats/Excel/Templates/Confidence Interval for One Proportion.xlsx
@@ -1,35 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elucid\Desktop\Classes\Repos\General\Stats\Excel\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccasement\Dropbox (Fairfield University)\MATH 2217 - Statistics I\Excel Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC26B5D-0CC0-43E0-BE56-D3791632EBE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1970" yWindow="2760" windowWidth="18000" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -74,7 +62,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,20 +404,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
@@ -439,12 +425,12 @@
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
@@ -454,12 +440,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="2">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
@@ -468,13 +454,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="1">
         <f>C4/C5</f>
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
@@ -483,12 +469,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="2">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="E8" t="s">
         <v>3</v>
@@ -497,13 +483,13 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="1">
         <f>NORMINV(C8+(1-C8)/2,0,1)</f>
-        <v>1.6448536269514715</v>
+        <v>1.9599639845400536</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
@@ -513,13 +499,13 @@
         <v>1.9599639845400536</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="1">
         <f>SQRT(C6*(1-C6)/C5)</f>
-        <v>3.0199337741083E-2</v>
+        <v>5.656854249492381E-2</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
@@ -529,13 +515,13 @@
         <v>5.656854249492381E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="1">
         <f>C9*C10</f>
-        <v>4.9673490214952834E-2</v>
+        <v>0.11087230594797422</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
@@ -545,13 +531,13 @@
         <v>0.11087230594797422</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1">
         <f>C6-C11</f>
-        <v>0.19032650978504717</v>
+        <v>8.9127694052025794E-2</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
@@ -561,13 +547,13 @@
         <v>8.9127694052025794E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="1">
         <f>C6+C11</f>
-        <v>0.28967349021495281</v>
+        <v>0.31087230594797421</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>

</xml_diff>